<commit_message>
Added some code for Tethys
</commit_message>
<xml_diff>
--- a/SpermWhales/GofAK_FishingVessels_SpermWhales.xlsx
+++ b/SpermWhales/GofAK_FishingVessels_SpermWhales.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>Encounter</t>
   </si>
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -106,10 +106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,6 +574,18 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2">
+        <v>43701.288888888892</v>
+      </c>
+      <c r="H7" s="2">
+        <v>43701.314375000002</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">

</xml_diff>

<commit_message>
Added Encounter 2 - See
</commit_message>
<xml_diff>
--- a/SpermWhales/GofAK_FishingVessels_SpermWhales.xlsx
+++ b/SpermWhales/GofAK_FishingVessels_SpermWhales.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Encounter</t>
   </si>
@@ -393,7 +393,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,11 +476,11 @@
       <c r="F3" s="3">
         <v>43665.614606481482</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
+      <c r="G3" s="2">
+        <v>43665.502337962964</v>
+      </c>
+      <c r="H3" s="2">
+        <v>43665.605752314812</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>